<commit_message>
add beelingua di  reminder pembayaran
</commit_message>
<xml_diff>
--- a/public/assets/excel/reminderPembayaranImport.xlsx
+++ b/public/assets/excel/reminderPembayaranImport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\blash-piutang\public\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEA9C69-880D-48FD-B8A0-274B642A1FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E67677B-B53A-41D5-B7E6-90C8E0DF7BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6A3BD53F-5BCB-40A2-9A9E-527F39B9120B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Student ID</t>
   </si>
@@ -231,15 +231,33 @@
   </si>
   <si>
     <t>Keberhasilan pengisian KRS akan membentuk tagihan Full SKS yang wajib dibayarkan dalam waktu 1x24 jam</t>
+  </si>
+  <si>
+    <t>(1)
+Beelingua Fee</t>
+  </si>
+  <si>
+    <t>(1)
+Jatem Beelingua</t>
+  </si>
+  <si>
+    <t>(2)
+Beelingua Fee</t>
+  </si>
+  <si>
+    <t>(2)
+Jatem Beelingua</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -343,12 +361,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -395,8 +414,16 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95505C7A-A71B-4809-83F9-1830209E47E7}">
-  <dimension ref="A1:AS3"/>
+  <dimension ref="A1:AW3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -731,34 +758,37 @@
     <col min="12" max="13" width="12.6640625" customWidth="1"/>
     <col min="14" max="14" width="16.5546875" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="18.109375" customWidth="1"/>
-    <col min="24" max="24" width="17.88671875" customWidth="1"/>
-    <col min="25" max="27" width="16.6640625" customWidth="1"/>
-    <col min="28" max="28" width="18" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="14.88671875" customWidth="1"/>
-    <col min="31" max="32" width="12.109375" customWidth="1"/>
-    <col min="33" max="34" width="12.6640625" customWidth="1"/>
-    <col min="35" max="35" width="17" customWidth="1"/>
-    <col min="36" max="36" width="12.6640625" customWidth="1"/>
-    <col min="37" max="37" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14" customWidth="1"/>
-    <col min="40" max="40" width="15" customWidth="1"/>
-    <col min="41" max="41" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12" customWidth="1"/>
-    <col min="43" max="43" width="11.6640625" customWidth="1"/>
-    <col min="44" max="44" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.109375" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="18.109375" customWidth="1"/>
+    <col min="25" max="26" width="17.88671875" customWidth="1"/>
+    <col min="27" max="29" width="16.6640625" customWidth="1"/>
+    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="14.88671875" customWidth="1"/>
+    <col min="33" max="34" width="12.109375" customWidth="1"/>
+    <col min="35" max="36" width="12.6640625" customWidth="1"/>
+    <col min="37" max="37" width="17" customWidth="1"/>
+    <col min="38" max="38" width="12.6640625" customWidth="1"/>
+    <col min="39" max="39" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" customWidth="1"/>
+    <col min="43" max="43" width="15" customWidth="1"/>
+    <col min="44" max="44" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12" customWidth="1"/>
+    <col min="46" max="46" width="11.6640625" customWidth="1"/>
+    <col min="47" max="47" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.109375" customWidth="1"/>
+    <col min="49" max="49" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="11" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1">
+    <row r="1" spans="1:49" s="11" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -804,98 +834,110 @@
       <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AO1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AP1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AR1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AS1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AT1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="12" t="s">
+      <c r="AU1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AV1" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="AW1" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:45" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="2" spans="1:49" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -941,85 +983,97 @@
       <c r="O2" s="9">
         <v>0</v>
       </c>
-      <c r="P2" s="9">
-        <f>SUM(H2:O2)</f>
-        <v>19300000</v>
-      </c>
-      <c r="Q2" s="5">
+      <c r="P2" s="17">
+        <v>1600000</v>
+      </c>
+      <c r="Q2" s="9">
+        <f>SUM(H2:P2)</f>
+        <v>20900000</v>
+      </c>
+      <c r="R2" s="5">
         <v>44860</v>
       </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="5">
+      <c r="S2" s="6"/>
+      <c r="T2" s="5">
         <v>44888</v>
       </c>
-      <c r="T2" s="5">
+      <c r="U2" s="5">
         <v>44994</v>
       </c>
-      <c r="U2" s="6"/>
       <c r="V2" s="6"/>
-      <c r="W2" s="5">
+      <c r="W2" s="6"/>
+      <c r="X2" s="5">
         <v>44888</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="15" t="s">
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="5">
+        <v>44888</v>
+      </c>
+      <c r="AA2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="AB2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="7" t="s">
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" s="9">
+      <c r="AE2" s="9">
         <v>7300000</v>
       </c>
-      <c r="AD2" s="9">
+      <c r="AF2" s="9">
         <v>0</v>
       </c>
-      <c r="AE2" s="9">
+      <c r="AG2" s="9">
         <v>5200000</v>
       </c>
-      <c r="AF2" s="9">
+      <c r="AH2" s="9">
         <v>5200000</v>
       </c>
-      <c r="AG2" s="9">
+      <c r="AI2" s="9">
         <v>0</v>
-      </c>
-      <c r="AH2" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="9">
-        <v>1600000</v>
       </c>
       <c r="AJ2" s="9">
         <v>0</v>
       </c>
       <c r="AK2" s="9">
-        <f t="shared" ref="AK2" si="0">X2+AC2+AE2+AI2+AJ2</f>
-        <v>14100000</v>
-      </c>
-      <c r="AL2" s="5">
+        <v>1600000</v>
+      </c>
+      <c r="AL2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="9">
+        <v>1600000</v>
+      </c>
+      <c r="AN2" s="9">
+        <f>Y2+AE2+AG2+AK2+AL2+AM2</f>
+        <v>15700000</v>
+      </c>
+      <c r="AO2" s="5">
         <v>44860</v>
       </c>
-      <c r="AM2" s="6"/>
-      <c r="AN2" s="5">
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="5">
         <v>44888</v>
       </c>
-      <c r="AO2" s="5">
+      <c r="AR2" s="5">
         <v>44994</v>
       </c>
-      <c r="AP2" s="6"/>
-      <c r="AQ2" s="6"/>
-      <c r="AR2" s="5">
+      <c r="AS2" s="6"/>
+      <c r="AT2" s="6"/>
+      <c r="AU2" s="5">
         <v>44888</v>
       </c>
-      <c r="AS2" s="6"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="5">
+        <v>44888</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" ht="15" thickTop="1"/>
+    <row r="3" spans="1:49" ht="15" thickTop="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{BFD1A41E-EA52-405A-B01A-529682EF0EF6}"/>
+    <hyperlink ref="AA2" r:id="rId1" xr:uid="{BFD1A41E-EA52-405A-B01A-529682EF0EF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>